<commit_message>
Updated Automation task allocation
</commit_message>
<xml_diff>
--- a/Mars Standard Tasks.xlsx
+++ b/Mars Standard Tasks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell Latitude\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IndustryConnect\AdvancedTask\Task3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7DF29D-00FC-4A56-B8CF-0D9B9B7126AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067FC2D2-8567-49B1-BD54-20DC2009DB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27645" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Tasks" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="79">
   <si>
     <t xml:space="preserve">  Task</t>
   </si>
@@ -823,7 +823,7 @@
   </sheetPr>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -2409,8 +2409,8 @@
   </sheetPr>
   <dimension ref="A1:V1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2490,6 +2490,9 @@
       <c r="B3" t="s">
         <v>34</v>
       </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2498,6 +2501,9 @@
       <c r="B4" t="s">
         <v>34</v>
       </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -2506,6 +2512,9 @@
       <c r="B5" t="s">
         <v>34</v>
       </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -2514,6 +2523,9 @@
       <c r="B6" t="s">
         <v>34</v>
       </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -2522,6 +2534,9 @@
       <c r="B7" t="s">
         <v>34</v>
       </c>
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -2530,6 +2545,9 @@
       <c r="B8" t="s">
         <v>34</v>
       </c>
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -2538,6 +2556,9 @@
       <c r="B9" t="s">
         <v>34</v>
       </c>
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -2546,6 +2567,9 @@
       <c r="B10" t="s">
         <v>34</v>
       </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -2554,6 +2578,9 @@
       <c r="B11" t="s">
         <v>34</v>
       </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -2562,6 +2589,9 @@
       <c r="B12" t="s">
         <v>34</v>
       </c>
+      <c r="C12" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -2570,6 +2600,9 @@
       <c r="B13" t="s">
         <v>34</v>
       </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -2578,6 +2611,9 @@
       <c r="B14" t="s">
         <v>34</v>
       </c>
+      <c r="C14" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -2601,55 +2637,73 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
       <c r="B20" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
       <c r="B22" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -2657,7 +2711,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -2665,7 +2719,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -2673,7 +2727,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -2681,7 +2735,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -2689,11 +2743,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update excel task allocation file
</commit_message>
<xml_diff>
--- a/Mars Standard Tasks.xlsx
+++ b/Mars Standard Tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IndustryConnect\AdvancedTask\Task3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067FC2D2-8567-49B1-BD54-20DC2009DB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{24502D96-8550-415A-8C24-053F4506545C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27645" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-180" yWindow="-18120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Tasks" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="82">
   <si>
     <t xml:space="preserve">  Task</t>
   </si>
@@ -278,6 +278,15 @@
   </si>
   <si>
     <t>Spriti</t>
+  </si>
+  <si>
+    <t>Heather</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>Jyoti</t>
   </si>
 </sst>
 </file>
@@ -464,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -491,6 +500,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -853,12 +864,12 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="20" t="str">
+      <c r="F1" s="22" t="str">
         <f>HYPERLINK("https://docs.google.com/document/d/1crUJuzOtaxP2fNaX4ipazLL3rvBrlcDSKbTdXBV7oU0","How to run Mars webiste using Docker")</f>
         <v>How to run Mars webiste using Docker</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -887,9 +898,9 @@
       <c r="C2" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -901,9 +912,9 @@
       <c r="C3" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -915,9 +926,9 @@
       <c r="C4" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -929,9 +940,9 @@
       <c r="C5" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -943,9 +954,9 @@
       <c r="C6" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -957,9 +968,9 @@
       <c r="C7" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -971,9 +982,9 @@
       <c r="C8" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -985,9 +996,9 @@
       <c r="C9" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -2410,7 +2421,7 @@
   <dimension ref="A1:V1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2422,10 +2433,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="23"/>
       <c r="C1" s="5" t="s">
         <v>32</v>
       </c>
@@ -2463,7 +2474,9 @@
         <v>1</v>
       </c>
       <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="D2" s="20" t="s">
+        <v>80</v>
+      </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -2493,6 +2506,9 @@
       <c r="C3" t="s">
         <v>78</v>
       </c>
+      <c r="D3" s="21">
+        <v>45020</v>
+      </c>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2504,6 +2520,9 @@
       <c r="C4" t="s">
         <v>78</v>
       </c>
+      <c r="D4" s="21">
+        <v>45020</v>
+      </c>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -2513,7 +2532,10 @@
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="D5" s="21">
+        <v>45020</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2524,7 +2546,10 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="D6" s="21">
+        <v>45020</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2537,6 +2562,9 @@
       <c r="C7" t="s">
         <v>77</v>
       </c>
+      <c r="D7" s="21">
+        <v>45020</v>
+      </c>
     </row>
     <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -2546,7 +2574,10 @@
         <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>81</v>
+      </c>
+      <c r="D8" s="21">
+        <v>45020</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2559,6 +2590,9 @@
       <c r="C9" t="s">
         <v>77</v>
       </c>
+      <c r="D9" s="21">
+        <v>45020</v>
+      </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -2570,6 +2604,9 @@
       <c r="C10" t="s">
         <v>75</v>
       </c>
+      <c r="D10" s="21">
+        <v>45020</v>
+      </c>
     </row>
     <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -2581,6 +2618,9 @@
       <c r="C11" t="s">
         <v>75</v>
       </c>
+      <c r="D11" s="21">
+        <v>45020</v>
+      </c>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -2592,6 +2632,9 @@
       <c r="C12" t="s">
         <v>76</v>
       </c>
+      <c r="D12" s="21">
+        <v>45020</v>
+      </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -2603,6 +2646,9 @@
       <c r="C13" t="s">
         <v>76</v>
       </c>
+      <c r="D13" s="21">
+        <v>45020</v>
+      </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -2612,7 +2658,10 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>81</v>
+      </c>
+      <c r="D14" s="21">
+        <v>45020</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2710,6 +2759,9 @@
       <c r="B23" t="s">
         <v>34</v>
       </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -2718,6 +2770,9 @@
       <c r="B24" t="s">
         <v>34</v>
       </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -2725,6 +2780,9 @@
       </c>
       <c r="B25" t="s">
         <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3967,13 +4025,13 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
@@ -5082,11 +5140,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>

</xml_diff>

<commit_message>
Mars Standard task Updated
</commit_message>
<xml_diff>
--- a/Mars Standard Tasks.xlsx
+++ b/Mars Standard Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IndustryConnect\AdvancedTask\Task3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24502D96-8550-415A-8C24-053F4506545C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6ED254-4B0A-4A16-81A8-694F6F8239BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="-18120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-180" yWindow="-18120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Tasks" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="82">
   <si>
     <t xml:space="preserve">  Task</t>
   </si>
@@ -2420,8 +2420,8 @@
   </sheetPr>
   <dimension ref="A1:V1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3798,7 +3798,9 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3831,6 +3833,12 @@
       <c r="B2" t="s">
         <v>36</v>
       </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -3839,6 +3847,12 @@
       <c r="B3" t="s">
         <v>36</v>
       </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -3847,6 +3861,12 @@
       <c r="B4" t="s">
         <v>36</v>
       </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -3855,6 +3875,12 @@
       <c r="B5" t="s">
         <v>36</v>
       </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3863,6 +3889,12 @@
       <c r="B6" t="s">
         <v>36</v>
       </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -3871,6 +3903,12 @@
       <c r="B7" t="s">
         <v>36</v>
       </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -3879,6 +3917,12 @@
       <c r="B8" t="s">
         <v>36</v>
       </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -3887,6 +3931,12 @@
       <c r="B9" t="s">
         <v>36</v>
       </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -3895,6 +3945,12 @@
       <c r="B10" t="s">
         <v>36</v>
       </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -3903,6 +3959,12 @@
       <c r="B11" t="s">
         <v>36</v>
       </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -3911,6 +3973,12 @@
       <c r="B12" t="s">
         <v>36</v>
       </c>
+      <c r="C12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -3919,6 +3987,12 @@
       <c r="B13" t="s">
         <v>36</v>
       </c>
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -3927,6 +4001,12 @@
       <c r="B14" t="s">
         <v>36</v>
       </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -3935,6 +4015,12 @@
       <c r="B15" t="s">
         <v>36</v>
       </c>
+      <c r="C15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -3943,6 +4029,12 @@
       <c r="B16" t="s">
         <v>36</v>
       </c>
+      <c r="C16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -3951,6 +4043,12 @@
       <c r="B17" t="s">
         <v>36</v>
       </c>
+      <c r="C17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -3959,6 +4057,12 @@
       <c r="B18" t="s">
         <v>36</v>
       </c>
+      <c r="C18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -3967,6 +4071,12 @@
       <c r="B19" t="s">
         <v>36</v>
       </c>
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -3975,6 +4085,12 @@
       <c r="B20" t="s">
         <v>36</v>
       </c>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -3983,6 +4099,12 @@
       <c r="B21" t="s">
         <v>36</v>
       </c>
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -3991,6 +4113,12 @@
       <c r="B22" t="s">
         <v>36</v>
       </c>
+      <c r="C22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -3999,6 +4127,12 @@
       <c r="B23" t="s">
         <v>36</v>
       </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="21">
+        <v>45037</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -4006,6 +4140,12 @@
       </c>
       <c r="B24" t="s">
         <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="21">
+        <v>45037</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>